<commit_message>
verigen : AddDefine 함수 추가
</commit_message>
<xml_diff>
--- a/Common/doc/verigen/media/instruction_macros.xlsx
+++ b/Common/doc/verigen/media/instruction_macros.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\Profiles\Common\doc\verigen\media\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B51ED72-B887-46AC-86E9-04F60E4EF72F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C6FB58F-E353-43DB-9C8F-A117541A3EA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6000" yWindow="330" windowWidth="18390" windowHeight="15300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="390" windowWidth="28830" windowHeight="12150" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="summary" sheetId="6" r:id="rId1"/>
     <sheet name="_V" sheetId="17" r:id="rId2"/>
+    <sheet name="AddDefine" sheetId="18" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="27">
   <si>
     <t>함수 원형</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -109,6 +110,44 @@
   </si>
   <si>
     <t>function</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>function AddDefine(name, val)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>-</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>코드내에서 적용될 전역 정의 변수를 지정합니다.
+아래의 함수 또는 지정된 code 내용에 적용됩니다.
+module:add_code, module.apply_code, module.code</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>정의 변수 이름 (재정의 가능)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>val</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>정의 변수 값 (number 또는 string)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AddDefine</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>전역 정의 선언</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -440,9 +479,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63D1552F-D2B8-4AD9-9ECE-3CAF9162E459}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
@@ -470,6 +511,17 @@
       </c>
       <c r="C2" t="s">
         <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -483,7 +535,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90D60330-BA3B-4597-B119-0C80BCDA160E}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
@@ -544,4 +598,65 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C1A4A3E-FD06-4035-A68C-3884BD4805FB}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.125" customWidth="1"/>
+    <col min="2" max="2" width="55.875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
verigen 에 vfunction 추가
</commit_message>
<xml_diff>
--- a/Common/doc/verigen/media/instruction_macros.xlsx
+++ b/Common/doc/verigen/media/instruction_macros.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\Profiles\Common\doc\verigen\media\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A34F343-5833-406D-9BCC-AD60526AAF7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B67C5996-98D2-44A6-86FA-EB73D22117E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="390" windowWidth="28830" windowHeight="12150" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="768" yWindow="768" windowWidth="19068" windowHeight="10212" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="summary" sheetId="6" r:id="rId1"/>
     <sheet name="_V" sheetId="17" r:id="rId2"/>
+    <sheet name="vfunction" sheetId="18" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="29">
   <si>
     <t>함수 원형</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -109,6 +110,50 @@
   </si>
   <si>
     <t>function</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>vfunction</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>verilog 내 사용 함수 선언</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>구분</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>표현식</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>function vfunction(name, func)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>func</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>verilog에서 사용할 lua function</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>verilog 내에서 사용할 함수 이름.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>-</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>verilog 내에서 "$함수(...)" 로 lua 함수를 호출할 수 있습니다.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -440,19 +485,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63D1552F-D2B8-4AD9-9ECE-3CAF9162E459}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="10.25" customWidth="1"/>
-    <col min="3" max="3" width="33.625" customWidth="1"/>
+    <col min="1" max="1" width="10.19921875" customWidth="1"/>
+    <col min="3" max="3" width="33.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -463,7 +508,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -472,6 +517,17 @@
       </c>
       <c r="C2" t="s">
         <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -489,13 +545,13 @@
       <selection sqref="A1:B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="10.125" customWidth="1"/>
-    <col min="2" max="2" width="55.875" customWidth="1"/>
+    <col min="1" max="1" width="10.09765625" customWidth="1"/>
+    <col min="2" max="2" width="55.8984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -503,7 +559,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -511,7 +567,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="82.5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" ht="69.599999999999994" x14ac:dyDescent="0.4">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -519,7 +575,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
@@ -527,7 +583,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
@@ -535,7 +591,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
@@ -548,4 +604,72 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CD2A0D6-F503-4889-951F-97AA556AF750}">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="10.09765625" customWidth="1"/>
+    <col min="2" max="2" width="55.8984375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
fix verigen example and doc.
</commit_message>
<xml_diff>
--- a/Common/doc/verigen/media/instruction_macros.xlsx
+++ b/Common/doc/verigen/media/instruction_macros.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\Profiles\Common\doc\verigen\media\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEB069B3-C820-4ED3-8735-BC7C656446B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B65470C-DBC0-4ABF-8A32-3AB91B44340C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1515" yWindow="315" windowWidth="25725" windowHeight="15285" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="summary" sheetId="6" r:id="rId1"/>
@@ -42,19 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="68">
-  <si>
-    <t>함수 원형</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>반환값</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>설명</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="81">
   <si>
     <t>Type</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -92,27 +80,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>시작 값</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>문자열 확장 조작</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>끝 값 (생략할 경우 start 값과 동일하게 취급합니다.)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>증가 값 (생략할 경우 1또는 -1씩 증감 합니다. end-start 값의 부호에 따라.)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>문장을 start 에서 end 까지 step 만큼 증가시켜, 문장을 확장합니다.
-만약 문장이 $(…) 로 구현된 부분이 있다면 해당 부분만, 확장합니다. 없을 경우 전체 문장을 확장하며, 문장내 '#' 문자는 start 에서 end 까지 반복되는 값이 대입됩니다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>function</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -121,18 +88,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>verilog 내 사용 함수 선언</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>구분</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>표현식</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>name</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -145,54 +100,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>verilog에서 사용할 lua function</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>verilog 내에서 사용할 함수 이름.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>-</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>verilog 내에서 "$함수(...)" 로 lua 함수를 호출할 수 있습니다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>LOG2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>log2(X) 값을 반환한다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>DEMUX_BY_EN</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>demux 구현 template</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>RANGE</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>verilog range 구현 template</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MULTICYCLE</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>multicycle 구현 template</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>number</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -201,10 +112,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>log2 입력 값</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>$LOG2(val, [bOverflow])</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -213,65 +120,30 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>log2(val) 값을 반환한다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>val 은 2^N 에 해당하는 정수 이어야 합니다.
-그렇지 않을 경우 에러를 반환합니다.
-결과 값에 대해 강제로 반올림 처리가 필요할 경우 이 값을 true 로 지정합니다.
-생략할 경우 false 로 간주합니다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>$DEMUX_BY_EN(width, channel_count, en, data_in, data_out)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>demux_by_enable 모듈을 이용하여, demux를 구현합니다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>width</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>1개 data 당 bitwidth</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>channel_count</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>입력 채널 개수</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>en</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>입력 enable 신호(string)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>data_in</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>입력 데이터 (총 channel_count 개수 만큼, string)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>data_out</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>출력 데이터 (string)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>$MULTICYCLE(module_inst_name, if_name, cycle_count, [instance_count], [clk])</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -280,10 +152,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>현재 모듈의 하위에 포함된 모듈 이름</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>if_name</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -300,16 +168,189 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>multicycle 구현 template "MultiCyclePath" 모듈 또는 "MultiCyclePathEx"를 이용하여, interface 1개인 모듈을 multicycle로 구현한다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>module_inst_name 의 모듈에 대응하는 interface instance 명을 지정합니다.</t>
+    <t>$LOG2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>$RANGE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>$DEMUX_BY_EN</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>$MULTICYCLE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>$add_interface</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>$set_param</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>$_V</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>$add_clock</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>$set_author</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>$set_inception</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Refer to @&lt;bookmark:@module:set_author&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>verilog bitwidth range template</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>demux design template</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>multicycle design template</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>log2(X) function</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Refer to @&lt;bookmark:@_V macro&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Refer to @&lt;bookmark:@module:set_inception&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Refer to @&lt;bookmark:@module:set_param&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Refer to @&lt;bookmark:@module:add_interface&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Refer to @&lt;bookmark:@module:add_clock&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Prototype</t>
+  </si>
+  <si>
+    <t>Prototype</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>string expansion manipulation</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Declaring a function for verilog</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Return value</t>
+  </si>
+  <si>
+    <t>Return value</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Remarks</t>
+  </si>
+  <si>
+    <t>Remarks</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Extends a statement by incrementing it by a step from start to end.
+If there is a part of the statement implemented with $(…), only that part is expanded. If there is none, the entire sentence is expanded, and the '#' character in the sentence is assigned a repeated value from start to end.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>start value</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>end value (If omitted, it is treated the same as the start value.)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>increase value (If omitted, it increases or decreases by 1 or -1. according to the sign of the end-start value.)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>You can call lua functions from within verilog with "$function(...)".</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Returns log2(val) value.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>log2 input value</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>val must be an integer equal to 2^N .
+If not, return an error.
+Set this value to true to force rounding up on the resulting value.
+If omitted, false is assumed.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Implement demux using demux_by_enable module.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bitwidth per data</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Number of input channels</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>input enable signal (string)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Input data (as many as the total number of channel_count, string)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>output data (string)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Multicycle Implementation Using the template "MultiCyclePath" module or "MultiCyclePathEx", a module with one interface is implemented as multicycle.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Module name included as a child of the current module</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Specifies the interface instance name corresponding to the module of module_inst_name.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <r>
-      <t xml:space="preserve">cycle 수 (2 ≤ cycle_count </t>
+      <t xml:space="preserve">cycle count (2 ≤ cycle_count </t>
     </r>
     <r>
       <rPr>
@@ -334,13 +375,21 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>하위 모듈의 instance 수 (1 ≤ instance_count ≤ cycle_count)
-생략할 경우 cycle_count 와 동일한 수로 간주한다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>multicycle 구현에 사용할 클럭
-생략할 경우 default clock 을 사용한다. (clock:set_default() 함수 참조)</t>
+    <t>Number of instances of submodules (1 ≤ instance_count ≤ cycle_count)
+If omitted, it is regarded as the same number as cycle_count.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Clock to use for multicycle implementation
+If omitted, the default clock is used. (see @&lt;bookmark:clock:set_default&gt;() function)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>lua function to use in verilog</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Function name to use within verilog</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -682,7 +731,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C3"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -693,35 +742,35 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>13</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>19</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -733,11 +782,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42D08EB2-AEB8-4165-9865-D902BB6CB17B}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
@@ -747,57 +794,123 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>30</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
         <v>35</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="B7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>36</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>40</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>39</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>37</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -808,10 +921,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90D60330-BA3B-4597-B119-0C80BCDA160E}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B3"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -824,48 +937,56 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>8</v>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>1</v>
+        <v>52</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="82.5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:2" ht="99" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" t="s">
-        <v>12</v>
+        <v>58</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>14</v>
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" t="s">
-        <v>15</v>
+        <v>7</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -879,8 +1000,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CD2A0D6-F503-4889-951F-97AA556AF750}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -891,50 +1012,50 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>21</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>0</v>
+        <v>51</v>
       </c>
       <c r="B2" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>1</v>
+        <v>55</v>
       </c>
       <c r="B3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="33" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>2</v>
+        <v>57</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>28</v>
+        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>26</v>
+        <v>80</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>25</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -949,7 +1070,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B5"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -960,50 +1081,50 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>21</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>0</v>
+        <v>51</v>
       </c>
       <c r="B2" t="s">
-        <v>40</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>1</v>
+        <v>56</v>
       </c>
       <c r="B3" t="s">
-        <v>37</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>2</v>
+        <v>57</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>42</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>38</v>
+        <v>16</v>
       </c>
       <c r="B5" t="s">
-        <v>39</v>
+        <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="82.5" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>41</v>
+        <v>18</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>43</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -1018,7 +1139,7 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B4"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1029,74 +1150,74 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>21</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>0</v>
+        <v>51</v>
       </c>
       <c r="B2" t="s">
-        <v>44</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>1</v>
+        <v>56</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>2</v>
+        <v>57</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>45</v>
+        <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>46</v>
+        <v>20</v>
       </c>
       <c r="B5" t="s">
-        <v>47</v>
+        <v>68</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>48</v>
+        <v>21</v>
       </c>
       <c r="B6" t="s">
-        <v>49</v>
+        <v>69</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>50</v>
+        <v>22</v>
       </c>
       <c r="B7" t="s">
-        <v>51</v>
+        <v>70</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>52</v>
+        <v>23</v>
       </c>
       <c r="B8" t="s">
-        <v>53</v>
+        <v>71</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>54</v>
+        <v>24</v>
       </c>
       <c r="B9" t="s">
-        <v>55</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -1110,8 +1231,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D468176-F76C-43B0-BF10-A41E7C9E9FF1}">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1122,78 +1243,79 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>21</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>0</v>
+        <v>51</v>
       </c>
       <c r="B2" t="s">
-        <v>56</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>1</v>
+        <v>56</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>2</v>
+        <v>57</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>63</v>
+        <v>73</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>57</v>
+        <v>26</v>
       </c>
       <c r="B5" t="s">
-        <v>58</v>
+        <v>74</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>59</v>
+        <v>27</v>
       </c>
       <c r="B6" t="s">
-        <v>64</v>
+        <v>75</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>60</v>
+        <v>28</v>
       </c>
       <c r="B7" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="33" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>61</v>
+        <v>29</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>62</v>
+        <v>30</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>67</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
verigen 에 lua 리스트 추가
</commit_message>
<xml_diff>
--- a/Common/doc/verigen/media/instruction_macros.xlsx
+++ b/Common/doc/verigen/media/instruction_macros.xlsx
@@ -1,25 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\Profiles\Common\doc\verigen\media\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B65470C-DBC0-4ABF-8A32-3AB91B44340C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9837FDA-7FC1-4098-B6B6-105846EE003F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1515" yWindow="315" windowWidth="25725" windowHeight="15285" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4050" yWindow="1200" windowWidth="21405" windowHeight="14010" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="summary" sheetId="6" r:id="rId1"/>
     <sheet name="vfunction_list" sheetId="19" r:id="rId2"/>
     <sheet name="_V" sheetId="17" r:id="rId3"/>
     <sheet name="vfunction" sheetId="18" r:id="rId4"/>
-    <sheet name="LOG2" sheetId="20" r:id="rId5"/>
-    <sheet name="DEMUX_BY_EN" sheetId="21" r:id="rId6"/>
-    <sheet name="MULTICYCLE" sheetId="22" r:id="rId7"/>
+    <sheet name="verigen_description" sheetId="23" r:id="rId5"/>
+    <sheet name="LOG2" sheetId="20" r:id="rId6"/>
+    <sheet name="DEMUX_BY_EN" sheetId="21" r:id="rId7"/>
+    <sheet name="MULTICYCLE" sheetId="22" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="87">
   <si>
     <t>Type</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -390,6 +391,30 @@
   </si>
   <si>
     <t>Function name to use within verilog</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>verigen_description</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Set verigen source code description</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>function verigen_description(desc)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Set verigen source's description in Lua file</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>desc</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>description of verigen source file</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -728,10 +753,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63D1552F-D2B8-4AD9-9ECE-3CAF9162E459}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -771,6 +796,17 @@
       </c>
       <c r="C3" t="s">
         <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -1000,8 +1036,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CD2A0D6-F503-4889-951F-97AA556AF750}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1066,6 +1102,64 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F2E7FFC-C690-4B53-A654-785B7C073B02}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.125" customWidth="1"/>
+    <col min="2" max="2" width="55.875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72CCA586-EDEA-4335-AAEA-5226888A1CF3}">
   <dimension ref="A1:B6"/>
   <sheetViews>
@@ -1134,7 +1228,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5683DEA-BC8E-4407-8E50-5A8B8183B0D9}">
   <dimension ref="A1:B9"/>
   <sheetViews>
@@ -1227,7 +1321,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D468176-F76C-43B0-BF10-A41E7C9E9FF1}">
   <dimension ref="A1:B9"/>
   <sheetViews>

</xml_diff>

<commit_message>
verigen 에 sub_module 객체 추가
</commit_message>
<xml_diff>
--- a/Common/doc/verigen/media/instruction_macros.xlsx
+++ b/Common/doc/verigen/media/instruction_macros.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\Profiles\Common\doc\verigen\media\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4173A96-F1F0-4328-BFA4-0035AD808731}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C85C82B6-307D-436C-9693-96F7752B569E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4050" yWindow="1200" windowWidth="21405" windowHeight="14010" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5025" yWindow="615" windowWidth="21405" windowHeight="14010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="summary" sheetId="6" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="92">
   <si>
     <t>Type</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -423,6 +423,18 @@
   </si>
   <si>
     <t>Refer to @&lt;bookmark:@module:add_code&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sub_module</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>data</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sub-module instance list</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -761,10 +773,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63D1552F-D2B8-4AD9-9ECE-3CAF9162E459}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -817,6 +829,17 @@
         <v>82</v>
       </c>
     </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>89</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C5" t="s">
+        <v>91</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -828,7 +851,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42D08EB2-AEB8-4165-9865-D902BB6CB17B}">
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>

</xml_diff>

<commit_message>
verigen 의 set_document 를 add_document 로 변경
</commit_message>
<xml_diff>
--- a/Common/doc/verigen/media/instruction_macros.xlsx
+++ b/Common/doc/verigen/media/instruction_macros.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\Profiles\Common\doc\verigen\media\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C85C82B6-307D-436C-9693-96F7752B569E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{284218E1-3E4F-46CF-96A8-CF69FE1E5690}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5025" yWindow="615" windowWidth="21405" windowHeight="14010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7005" yWindow="135" windowWidth="21405" windowHeight="15405" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="summary" sheetId="6" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="94">
   <si>
     <t>Type</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -435,6 +435,14 @@
   </si>
   <si>
     <t>Sub-module instance list</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>$add_document</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Refer to @&lt;bookmark:@module:add_document&gt;</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -775,7 +783,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63D1552F-D2B8-4AD9-9ECE-3CAF9162E459}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
@@ -849,9 +857,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42D08EB2-AEB8-4165-9865-D902BB6CB17B}">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
@@ -949,45 +959,56 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>36</v>
+        <v>92</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C9" t="s">
-        <v>48</v>
+        <v>93</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C11" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C12" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>37</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" t="s">
         <v>46</v>
       </c>
     </row>

</xml_diff>

<commit_message>
verigen 에 read_excel_table 함수 추가
</commit_message>
<xml_diff>
--- a/Common/doc/verigen/media/instruction_macros.xlsx
+++ b/Common/doc/verigen/media/instruction_macros.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\Profiles\Common\doc\verigen\media\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{284218E1-3E4F-46CF-96A8-CF69FE1E5690}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF9A7210-0542-4CE8-B382-4201148177A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7005" yWindow="135" windowWidth="21405" windowHeight="15405" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9075" yWindow="3615" windowWidth="19515" windowHeight="9705" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="summary" sheetId="6" r:id="rId1"/>
@@ -18,9 +18,10 @@
     <sheet name="_V" sheetId="17" r:id="rId3"/>
     <sheet name="vfunction" sheetId="18" r:id="rId4"/>
     <sheet name="verigen_description" sheetId="23" r:id="rId5"/>
-    <sheet name="LOG2" sheetId="20" r:id="rId6"/>
-    <sheet name="DEMUX_BY_EN" sheetId="21" r:id="rId7"/>
-    <sheet name="MULTICYCLE" sheetId="22" r:id="rId8"/>
+    <sheet name="read_excel_table" sheetId="24" r:id="rId6"/>
+    <sheet name="LOG2" sheetId="20" r:id="rId7"/>
+    <sheet name="DEMUX_BY_EN" sheetId="21" r:id="rId8"/>
+    <sheet name="MULTICYCLE" sheetId="22" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="107">
   <si>
     <t>Type</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -443,6 +444,58 @@
   </si>
   <si>
     <t>Refer to @&lt;bookmark:@module:add_document&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>read_excel_table</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Read excel sheet table to Lua array</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Lua 2D array</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Read excel table sheet to Lua table</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>file_name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sheet_name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Excel file's sheet name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Excel file name to read</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>function read_excel_table(file_name, sheet_name, [tag_name], [position…])</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>tag_name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Table's base tag name to set a table key [optional]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>position</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Specific table start position on sheet [optional], 'x,y' position or excel position(ex. "B3")</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -781,10 +834,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63D1552F-D2B8-4AD9-9ECE-3CAF9162E459}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -839,12 +892,23 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>94</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>89</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B6" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C6" t="s">
         <v>91</v>
       </c>
     </row>
@@ -859,7 +923,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42D08EB2-AEB8-4165-9865-D902BB6CB17B}">
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
@@ -1169,7 +1233,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F2E7FFC-C690-4B53-A654-785B7C073B02}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1220,10 +1286,93 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3F9441B-98E2-4944-AD65-46DEF14E0873}">
+  <dimension ref="A1:B8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.125" customWidth="1"/>
+    <col min="2" max="2" width="55.875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B3" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B5" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B6" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B7" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B8" t="s">
+        <v>106</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72CCA586-EDEA-4335-AAEA-5226888A1CF3}">
   <dimension ref="A1:B6"/>
   <sheetViews>
@@ -1292,7 +1441,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5683DEA-BC8E-4407-8E50-5A8B8183B0D9}">
   <dimension ref="A1:B9"/>
   <sheetViews>
@@ -1385,7 +1534,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D468176-F76C-43B0-BF10-A41E7C9E9FF1}">
   <dimension ref="A1:B9"/>
   <sheetViews>

</xml_diff>

<commit_message>
verigen에 verigen_add_reference 함수 추가
</commit_message>
<xml_diff>
--- a/Common/doc/verigen/media/instruction_macros.xlsx
+++ b/Common/doc/verigen/media/instruction_macros.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\Profiles\Common\doc\verigen\media\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF9A7210-0542-4CE8-B382-4201148177A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4836774D-F9E2-40C8-8103-F5519ECC7AC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9075" yWindow="3615" windowWidth="19515" windowHeight="9705" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="summary" sheetId="6" r:id="rId1"/>
@@ -18,10 +18,11 @@
     <sheet name="_V" sheetId="17" r:id="rId3"/>
     <sheet name="vfunction" sheetId="18" r:id="rId4"/>
     <sheet name="verigen_description" sheetId="23" r:id="rId5"/>
-    <sheet name="read_excel_table" sheetId="24" r:id="rId6"/>
-    <sheet name="LOG2" sheetId="20" r:id="rId7"/>
-    <sheet name="DEMUX_BY_EN" sheetId="21" r:id="rId8"/>
-    <sheet name="MULTICYCLE" sheetId="22" r:id="rId9"/>
+    <sheet name="verigen_add_reference" sheetId="25" r:id="rId6"/>
+    <sheet name="read_excel_table" sheetId="24" r:id="rId7"/>
+    <sheet name="LOG2" sheetId="20" r:id="rId8"/>
+    <sheet name="DEMUX_BY_EN" sheetId="21" r:id="rId9"/>
+    <sheet name="MULTICYCLE" sheetId="22" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -44,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="111">
   <si>
     <t>Type</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -496,6 +497,22 @@
   </si>
   <si>
     <t>Specific table start position on sheet [optional], 'x,y' position or excel position(ex. "B3")</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>function verigen_add_reference(filename, desc)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>filename</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>target source file name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Add link &amp; description to verigen top reference list</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -919,12 +936,105 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D468176-F76C-43B0-BF10-A41E7C9E9FF1}">
+  <dimension ref="A1:B9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.125" customWidth="1"/>
+    <col min="2" max="2" width="55.875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42D08EB2-AEB8-4165-9865-D902BB6CB17B}">
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="A10" sqref="A10:XFD10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1291,10 +1401,12 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3F9441B-98E2-4944-AD65-46DEF14E0873}">
-  <dimension ref="A1:B8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13AAA5BD-3EFD-4038-BB1B-9651D6550384}">
+  <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1315,7 +1427,7 @@
         <v>51</v>
       </c>
       <c r="B2" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -1323,7 +1435,7 @@
         <v>55</v>
       </c>
       <c r="B3" t="s">
-        <v>96</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -1331,39 +1443,23 @@
         <v>57</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>97</v>
+        <v>110</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="B5" t="s">
-        <v>101</v>
+        <v>108</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>99</v>
+        <v>85</v>
       </c>
       <c r="B6" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="B7" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="B8" t="s">
-        <v>106</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -1373,6 +1469,88 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3F9441B-98E2-4944-AD65-46DEF14E0873}">
+  <dimension ref="A1:B8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.125" customWidth="1"/>
+    <col min="2" max="2" width="55.875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B3" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B5" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B6" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B7" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B8" t="s">
+        <v>106</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72CCA586-EDEA-4335-AAEA-5226888A1CF3}">
   <dimension ref="A1:B6"/>
   <sheetViews>
@@ -1441,7 +1619,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5683DEA-BC8E-4407-8E50-5A8B8183B0D9}">
   <dimension ref="A1:B9"/>
   <sheetViews>
@@ -1532,97 +1710,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D468176-F76C-43B0-BF10-A41E7C9E9FF1}">
-  <dimension ref="A1:B9"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="10.125" customWidth="1"/>
-    <col min="2" max="2" width="55.875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="B2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="B3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B5" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B6" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B7" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>78</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
verigen 에 verigen_add_verilog 함수 추가
</commit_message>
<xml_diff>
--- a/Common/doc/verigen/media/instruction_macros.xlsx
+++ b/Common/doc/verigen/media/instruction_macros.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\Profiles\Common\doc\verigen\media\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4836774D-F9E2-40C8-8103-F5519ECC7AC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{565E586C-DEEF-4EE7-AB7D-BAE9B10C8AA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="summary" sheetId="6" r:id="rId1"/>
@@ -19,10 +19,11 @@
     <sheet name="vfunction" sheetId="18" r:id="rId4"/>
     <sheet name="verigen_description" sheetId="23" r:id="rId5"/>
     <sheet name="verigen_add_reference" sheetId="25" r:id="rId6"/>
-    <sheet name="read_excel_table" sheetId="24" r:id="rId7"/>
-    <sheet name="LOG2" sheetId="20" r:id="rId8"/>
-    <sheet name="DEMUX_BY_EN" sheetId="21" r:id="rId9"/>
-    <sheet name="MULTICYCLE" sheetId="22" r:id="rId10"/>
+    <sheet name="verigen_add_verilog" sheetId="26" r:id="rId7"/>
+    <sheet name="read_excel_table" sheetId="24" r:id="rId8"/>
+    <sheet name="LOG2" sheetId="20" r:id="rId9"/>
+    <sheet name="DEMUX_BY_EN" sheetId="21" r:id="rId10"/>
+    <sheet name="MULTICYCLE" sheetId="22" r:id="rId11"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -45,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="114">
   <si>
     <t>Type</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -513,6 +514,18 @@
   </si>
   <si>
     <t>Add link &amp; description to verigen top reference list</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Add verilog source(s)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>function verigen_add_verilog(filename)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>verilog file name (can use wildcard '*')</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -937,6 +950,99 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5683DEA-BC8E-4407-8E50-5A8B8183B0D9}">
+  <dimension ref="A1:B9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.125" customWidth="1"/>
+    <col min="2" max="2" width="55.875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" t="s">
+        <v>72</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D468176-F76C-43B0-BF10-A41E7C9E9FF1}">
   <dimension ref="A1:B9"/>
   <sheetViews>
@@ -1404,8 +1510,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13AAA5BD-3EFD-4038-BB1B-9651D6550384}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1465,10 +1571,70 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9A98FFF-B626-4BBF-94AB-7F94D0FECB5D}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.125" customWidth="1"/>
+    <col min="2" max="2" width="55.875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3F9441B-98E2-4944-AD65-46DEF14E0873}">
   <dimension ref="A1:B8"/>
   <sheetViews>
@@ -1550,7 +1716,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72CCA586-EDEA-4335-AAEA-5226888A1CF3}">
   <dimension ref="A1:B6"/>
   <sheetViews>
@@ -1617,97 +1783,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5683DEA-BC8E-4407-8E50-5A8B8183B0D9}">
-  <dimension ref="A1:B9"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="10.125" customWidth="1"/>
-    <col min="2" max="2" width="55.875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="B2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="B3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B5" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B6" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B7" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B8" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B9" t="s">
-        <v>72</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
verigen : add verigen_set_max_showlink() function
</commit_message>
<xml_diff>
--- a/Common/doc/verigen/media/instruction_macros.xlsx
+++ b/Common/doc/verigen/media/instruction_macros.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\Profiles\Common\doc\verigen\media\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{565E586C-DEEF-4EE7-AB7D-BAE9B10C8AA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25C2FF87-50FB-408F-BFB8-CA07C0C53B95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" firstSheet="3" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="summary" sheetId="6" r:id="rId1"/>
@@ -20,10 +20,11 @@
     <sheet name="verigen_description" sheetId="23" r:id="rId5"/>
     <sheet name="verigen_add_reference" sheetId="25" r:id="rId6"/>
     <sheet name="verigen_add_verilog" sheetId="26" r:id="rId7"/>
-    <sheet name="read_excel_table" sheetId="24" r:id="rId8"/>
-    <sheet name="LOG2" sheetId="20" r:id="rId9"/>
-    <sheet name="DEMUX_BY_EN" sheetId="21" r:id="rId10"/>
-    <sheet name="MULTICYCLE" sheetId="22" r:id="rId11"/>
+    <sheet name="verigen_set_max_showlink" sheetId="27" r:id="rId8"/>
+    <sheet name="read_excel_table" sheetId="24" r:id="rId9"/>
+    <sheet name="LOG2" sheetId="20" r:id="rId10"/>
+    <sheet name="DEMUX_BY_EN" sheetId="21" r:id="rId11"/>
+    <sheet name="MULTICYCLE" sheetId="22" r:id="rId12"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -46,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="118">
   <si>
     <t>Type</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -526,6 +527,24 @@
   </si>
   <si>
     <t>verilog file name (can use wildcard '*')</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>verigen_set_max_showlink(size)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>size</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Set design hierarchy tree's link count between the modules.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>maximum link count.
+If "size" is 0 or less, all connected links will be shown.
+(default value : 8)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -950,6 +969,75 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72CCA586-EDEA-4335-AAEA-5226888A1CF3}">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.125" customWidth="1"/>
+    <col min="2" max="2" width="55.875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="82.5" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5683DEA-BC8E-4407-8E50-5A8B8183B0D9}">
   <dimension ref="A1:B9"/>
   <sheetViews>
@@ -1042,7 +1130,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D468176-F76C-43B0-BF10-A41E7C9E9FF1}">
   <dimension ref="A1:B9"/>
   <sheetViews>
@@ -1579,7 +1667,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9A98FFF-B626-4BBF-94AB-7F94D0FECB5D}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1630,11 +1720,72 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CB4995A-8964-4370-9032-FF45D8391D6A}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.125" customWidth="1"/>
+    <col min="2" max="2" width="55.875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3F9441B-98E2-4944-AD65-46DEF14E0873}">
   <dimension ref="A1:B8"/>
   <sheetViews>
@@ -1714,73 +1865,4 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72CCA586-EDEA-4335-AAEA-5226888A1CF3}">
-  <dimension ref="A1:B6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="10.125" customWidth="1"/>
-    <col min="2" max="2" width="55.875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="B2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="B3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="82.5" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
veigen 에 기본 함수 verigen.~ 으로 변경
</commit_message>
<xml_diff>
--- a/Common/doc/verigen/media/instruction_macros.xlsx
+++ b/Common/doc/verigen/media/instruction_macros.xlsx
@@ -1,30 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Project\Profiles\Common\doc\verigen\media\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\Profiles\Common\doc\verigen\media\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCF4EB5C-89D5-42BF-B567-39B55B6267DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5848A006-7F36-40E5-8E45-E85B3407D326}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21020" yWindow="8440" windowWidth="17010" windowHeight="11830" firstSheet="6" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="4" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="summary" sheetId="6" r:id="rId1"/>
     <sheet name="vfunction_list" sheetId="19" r:id="rId2"/>
     <sheet name="_V" sheetId="17" r:id="rId3"/>
     <sheet name="vfunction" sheetId="18" r:id="rId4"/>
-    <sheet name="verigen_description" sheetId="23" r:id="rId5"/>
-    <sheet name="verigen_add_reference" sheetId="25" r:id="rId6"/>
-    <sheet name="verigen_add_verilog" sheetId="26" r:id="rId7"/>
-    <sheet name="verigen_set_max_showlink" sheetId="27" r:id="rId8"/>
-    <sheet name="read_excel_table" sheetId="24" r:id="rId9"/>
-    <sheet name="LOG2" sheetId="20" r:id="rId10"/>
-    <sheet name="DEMUX_BY_EN" sheetId="21" r:id="rId11"/>
-    <sheet name="MULTICYCLE" sheetId="22" r:id="rId12"/>
+    <sheet name="verigen.set_description" sheetId="23" r:id="rId5"/>
+    <sheet name="verigen.add_reference" sheetId="25" r:id="rId6"/>
+    <sheet name="verigen.add_verilog" sheetId="26" r:id="rId7"/>
+    <sheet name="verigen.set_max_showlink" sheetId="27" r:id="rId8"/>
+    <sheet name="verigen.set_constraint" sheetId="28" r:id="rId9"/>
+    <sheet name="read_excel_table" sheetId="24" r:id="rId10"/>
+    <sheet name="LOG2" sheetId="20" r:id="rId11"/>
+    <sheet name="DEMUX_BY_EN" sheetId="21" r:id="rId12"/>
+    <sheet name="MULTICYCLE" sheetId="22" r:id="rId13"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="129">
   <si>
     <t>Type</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -387,10 +388,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>verigen_description</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Set verigen source code description</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -516,10 +513,6 @@
   </si>
   <si>
     <t>verilog file name (can use wildcard '*')</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>verigen_set_max_showlink(size)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -533,23 +526,61 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>verigen_add_reference</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>verigen_add_verilog</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>verigen_set_max_showlink</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Set design hierarchy tree's maximum link count between the modules</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Set design hierarchy tree's maximum link count between the modules.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>verigen.set_max_showlink(size)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>verigen.set_max_showlink</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>verigen.add_verilog</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>verigen.set_description</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>verigen.add_reference</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>verigen.set_constraint</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Set constaint</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>verigen.set_constaint(name, constaint)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Set constaint for hardware design.
+If 'name' and 'constaint' is nil, then clear all constaint.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>constaint</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>constaint description</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>name of constaint
+If 'name' is nil, then add constaint to previous named constained. Previous same named constraint will be overwrited.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -888,19 +919,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63D1552F-D2B8-4AD9-9ECE-3CAF9162E459}">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10.25" customWidth="1"/>
-    <col min="3" max="3" width="33.58203125" customWidth="1"/>
+    <col min="3" max="3" width="33.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -911,7 +942,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -922,7 +953,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -933,70 +964,81 @@
         <v>54</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>81</v>
+        <v>120</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C7" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>94</v>
+        <v>122</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C8" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
+        <v>93</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>88</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="C10" t="s">
         <v>90</v>
-      </c>
-      <c r="C9" t="s">
-        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -1007,6 +1049,88 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3F9441B-98E2-4944-AD65-46DEF14E0873}">
+  <dimension ref="A1:B8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.125" customWidth="1"/>
+    <col min="2" max="2" width="55.875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B5" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B6" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B7" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B8" t="s">
+        <v>105</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72CCA586-EDEA-4335-AAEA-5226888A1CF3}">
   <dimension ref="A1:B6"/>
   <sheetViews>
@@ -1014,13 +1138,13 @@
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.08203125" customWidth="1"/>
-    <col min="2" max="2" width="55.83203125" customWidth="1"/>
+    <col min="1" max="1" width="10.125" customWidth="1"/>
+    <col min="2" max="2" width="55.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1028,7 +1152,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>51</v>
       </c>
@@ -1036,7 +1160,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>56</v>
       </c>
@@ -1044,7 +1168,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>57</v>
       </c>
@@ -1052,7 +1176,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>16</v>
       </c>
@@ -1060,105 +1184,12 @@
         <v>65</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="85" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:2" ht="82.5" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>66</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5683DEA-BC8E-4407-8E50-5A8B8183B0D9}">
-  <dimension ref="A1:B9"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
-  <cols>
-    <col min="1" max="1" width="10.08203125" customWidth="1"/>
-    <col min="2" max="2" width="55.83203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A2" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="B2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A3" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="B3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A4" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A5" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B5" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A6" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B6" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A7" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B7" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A8" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B8" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A9" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B9" t="s">
-        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -1169,6 +1200,99 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5683DEA-BC8E-4407-8E50-5A8B8183B0D9}">
+  <dimension ref="A1:B9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.125" customWidth="1"/>
+    <col min="2" max="2" width="55.875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" t="s">
+        <v>72</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D468176-F76C-43B0-BF10-A41E7C9E9FF1}">
   <dimension ref="A1:B9"/>
   <sheetViews>
@@ -1176,13 +1300,13 @@
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.08203125" customWidth="1"/>
-    <col min="2" max="2" width="55.83203125" customWidth="1"/>
+    <col min="1" max="1" width="10.125" customWidth="1"/>
+    <col min="2" max="2" width="55.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1190,7 +1314,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>51</v>
       </c>
@@ -1198,7 +1322,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>56</v>
       </c>
@@ -1206,7 +1330,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="51" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:2" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>57</v>
       </c>
@@ -1214,7 +1338,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>26</v>
       </c>
@@ -1222,7 +1346,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>27</v>
       </c>
@@ -1230,7 +1354,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>28</v>
       </c>
@@ -1238,7 +1362,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="51" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:2" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>29</v>
       </c>
@@ -1246,7 +1370,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="51" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:2" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>30</v>
       </c>
@@ -1269,13 +1393,13 @@
       <selection activeCell="A10" sqref="A10:XFD10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10.25" customWidth="1"/>
-    <col min="3" max="3" width="33.58203125" customWidth="1"/>
+    <col min="3" max="3" width="33.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -1286,7 +1410,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>31</v>
       </c>
@@ -1297,7 +1421,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>32</v>
       </c>
@@ -1308,7 +1432,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>33</v>
       </c>
@@ -1319,7 +1443,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>34</v>
       </c>
@@ -1330,7 +1454,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>38</v>
       </c>
@@ -1341,7 +1465,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>35</v>
       </c>
@@ -1352,29 +1476,29 @@
         <v>49</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C8" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C9" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>36</v>
       </c>
@@ -1385,7 +1509,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>40</v>
       </c>
@@ -1396,7 +1520,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>39</v>
       </c>
@@ -1407,7 +1531,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>37</v>
       </c>
@@ -1433,13 +1557,13 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.08203125" customWidth="1"/>
-    <col min="2" max="2" width="55.83203125" customWidth="1"/>
+    <col min="1" max="1" width="10.125" customWidth="1"/>
+    <col min="2" max="2" width="55.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1447,7 +1571,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>52</v>
       </c>
@@ -1455,7 +1579,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>55</v>
       </c>
@@ -1463,7 +1587,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="102" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:2" ht="99" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>58</v>
       </c>
@@ -1471,7 +1595,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -1479,7 +1603,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -1487,7 +1611,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
@@ -1510,13 +1634,13 @@
       <selection sqref="A1:B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.08203125" customWidth="1"/>
-    <col min="2" max="2" width="55.83203125" customWidth="1"/>
+    <col min="1" max="1" width="10.125" customWidth="1"/>
+    <col min="2" max="2" width="55.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1524,7 +1648,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>51</v>
       </c>
@@ -1532,7 +1656,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>55</v>
       </c>
@@ -1540,7 +1664,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:2" ht="33" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>57</v>
       </c>
@@ -1548,7 +1672,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
@@ -1556,7 +1680,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>13</v>
       </c>
@@ -1575,17 +1699,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F2E7FFC-C690-4B53-A654-785B7C073B02}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B5"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.08203125" customWidth="1"/>
-    <col min="2" max="2" width="55.83203125" customWidth="1"/>
+    <col min="1" max="1" width="10.125" customWidth="1"/>
+    <col min="2" max="2" width="55.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1593,15 +1715,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>51</v>
       </c>
       <c r="B2" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>55</v>
       </c>
@@ -1609,20 +1731,20 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>57</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A5" s="1" t="s">
+      <c r="B5" t="s">
         <v>85</v>
-      </c>
-      <c r="B5" t="s">
-        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -1640,13 +1762,13 @@
       <selection sqref="A1:B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.08203125" customWidth="1"/>
-    <col min="2" max="2" width="55.83203125" customWidth="1"/>
+    <col min="1" max="1" width="10.125" customWidth="1"/>
+    <col min="2" max="2" width="55.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1654,15 +1776,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>51</v>
       </c>
       <c r="B2" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>55</v>
       </c>
@@ -1670,28 +1792,28 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>57</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B6" t="s">
         <v>85</v>
-      </c>
-      <c r="B6" t="s">
-        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -1705,17 +1827,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9A98FFF-B626-4BBF-94AB-7F94D0FECB5D}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B5"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.08203125" customWidth="1"/>
-    <col min="2" max="2" width="55.83203125" customWidth="1"/>
+    <col min="1" max="1" width="10.125" customWidth="1"/>
+    <col min="2" max="2" width="55.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1723,15 +1843,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>51</v>
       </c>
       <c r="B2" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>55</v>
       </c>
@@ -1739,20 +1859,20 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>57</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
   </sheetData>
@@ -1766,17 +1886,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CB4995A-8964-4370-9032-FF45D8391D6A}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.08203125" customWidth="1"/>
-    <col min="2" max="2" width="55.83203125" customWidth="1"/>
+    <col min="1" max="1" width="10.125" customWidth="1"/>
+    <col min="2" max="2" width="55.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1784,15 +1904,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>51</v>
       </c>
       <c r="B2" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>55</v>
       </c>
@@ -1800,20 +1920,20 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="34" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:2" ht="33" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>57</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="51" x14ac:dyDescent="0.45">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
   </sheetData>
@@ -1824,18 +1944,20 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3F9441B-98E2-4944-AD65-46DEF14E0873}">
-  <dimension ref="A1:B8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75A529DA-237E-44AC-92D8-75163E62A239}">
+  <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.08203125" customWidth="1"/>
-    <col min="2" max="2" width="55.83203125" customWidth="1"/>
+    <col min="1" max="1" width="10.125" customWidth="1"/>
+    <col min="2" max="2" width="55.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1843,60 +1965,44 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>51</v>
       </c>
       <c r="B2" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>55</v>
       </c>
       <c r="B3" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="33" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>57</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="B5" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+        <v>11</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>99</v>
+        <v>126</v>
       </c>
       <c r="B6" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A7" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="B7" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A8" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="B8" t="s">
-        <v>106</v>
+        <v>127</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
verigen.set_max_showlink 기본값 5 로 수정
</commit_message>
<xml_diff>
--- a/Common/doc/verigen/media/instruction_macros.xlsx
+++ b/Common/doc/verigen/media/instruction_macros.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\Profiles\Common\doc\verigen\media\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5848A006-7F36-40E5-8E45-E85B3407D326}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A38BF7A2-2DDC-4E76-8C73-37A2A174E2BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="4" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3120" yWindow="2070" windowWidth="21465" windowHeight="13425" firstSheet="5" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="summary" sheetId="6" r:id="rId1"/>
@@ -520,67 +520,67 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>Set design hierarchy tree's maximum link count between the modules</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Set design hierarchy tree's maximum link count between the modules.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>verigen.set_max_showlink(size)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>verigen.set_max_showlink</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>verigen.add_verilog</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>verigen.set_description</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>verigen.add_reference</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>verigen.set_constraint</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Set constaint</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>verigen.set_constaint(name, constaint)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Set constaint for hardware design.
+If 'name' and 'constaint' is nil, then clear all constaint.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>constaint</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>constaint description</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>name of constaint
+If 'name' is nil, then add constaint to previous named constained. Previous same named constraint will be overwrited.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>maximum link count.
 If "size" is 0 or less, all connected links will be shown.
-(default value : 8)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Set design hierarchy tree's maximum link count between the modules</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Set design hierarchy tree's maximum link count between the modules.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>verigen.set_max_showlink(size)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>verigen.set_max_showlink</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>verigen.add_verilog</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>verigen.set_description</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>verigen.add_reference</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>verigen.set_constraint</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Set constaint</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>verigen.set_constaint(name, constaint)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Set constaint for hardware design.
-If 'name' and 'constaint' is nil, then clear all constaint.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>constaint</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>constaint description</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>name of constaint
-If 'name' is nil, then add constaint to previous named constained. Previous same named constraint will be overwrited.</t>
+(default value : 5)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -966,7 +966,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>9</v>
@@ -977,7 +977,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>9</v>
@@ -988,7 +988,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>9</v>
@@ -999,24 +999,24 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C8" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -1886,67 +1886,6 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CB4995A-8964-4370-9032-FF45D8391D6A}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="10.125" customWidth="1"/>
-    <col min="2" max="2" width="55.875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="B2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="B3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="33" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>114</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75A529DA-237E-44AC-92D8-75163E62A239}">
-  <dimension ref="A1:B6"/>
-  <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
@@ -1970,7 +1909,7 @@
         <v>51</v>
       </c>
       <c r="B2" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -1986,7 +1925,68 @@
         <v>57</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>125</v>
+        <v>115</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>128</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75A529DA-237E-44AC-92D8-75163E62A239}">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.125" customWidth="1"/>
+    <col min="2" max="2" width="55.875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="33" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="49.5" x14ac:dyDescent="0.3">
@@ -1994,15 +1994,15 @@
         <v>11</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B6" t="s">
         <v>126</v>
-      </c>
-      <c r="B6" t="s">
-        <v>127</v>
       </c>
     </row>
   </sheetData>

</xml_diff>